<commit_message>
global classroom allocation with proper tracking across all timetables
</commit_message>
<xml_diff>
--- a/backend/output_timetables/exam_schedule_20-11-2025_to_30-11-2025.xlsx
+++ b/backend/output_timetables/exam_schedule_20-11-2025_to_30-11-2025.xlsx
@@ -8,6 +8,10 @@
   </bookViews>
   <sheets>
     <sheet name="Exam_Schedule" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Exam_Classrooms" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Configuration" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Exam_Summary" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Department_Summary" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M42"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -499,6 +503,16 @@
           <t>status</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>classroom</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>capacity_info</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -562,6 +576,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -625,6 +649,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -688,6 +722,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -751,6 +795,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -814,6 +868,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -877,6 +941,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -940,6 +1014,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1003,6 +1087,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1066,6 +1160,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1129,6 +1233,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1192,6 +1306,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1255,6 +1379,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1318,6 +1452,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1381,6 +1525,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1444,6 +1598,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1507,6 +1671,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1570,6 +1744,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1633,6 +1817,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1696,6 +1890,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1759,6 +1963,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1822,6 +2036,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1885,6 +2109,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1948,6 +2182,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -2011,6 +2255,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -2074,6 +2328,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -2137,6 +2401,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -2200,6 +2474,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -2263,6 +2547,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -2326,6 +2620,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -2389,6 +2693,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2452,6 +2766,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2515,6 +2839,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2578,6 +2912,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2641,6 +2985,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2704,6 +3058,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2767,6 +3131,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2830,6 +3204,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2893,6 +3277,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2956,6 +3350,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -3019,6 +3423,16 @@
           <t>Scheduled</t>
         </is>
       </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -3081,6 +3495,2328 @@
         <is>
           <t>Scheduled</t>
         </is>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I42"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Course Code</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Course Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Session</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Time Slot</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Allocated Classrooms</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Estimated Enrollment</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Duration</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CS264</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Data Structures Lab</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>20-11-2025</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>CS101</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Programming Fundamentals</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>20-11-2025</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>DA261</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Statistical Programming</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>20-11-2025</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>CS304</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Artificial Intelligence</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>20-11-2025</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>EC101</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Electronics Theory</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>20-11-2025</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>CS263</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Data Structures</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>20-11-2025</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>MA161</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Statistics</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>20-11-2025</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>DA262</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Data Handling</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>20-11-2025</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>DS161</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Introduction to Programming</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>21-11-2025</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>MA261</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Differential Equations</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>21-11-2025</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CS307</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Machine Learning</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>21-11-2025</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>EC301</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Digital Signal Processing</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>21-11-2025</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>MA162</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Probability</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>21-11-2025</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>MA262</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Multivariable Calculus</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>21-11-2025</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>EC302</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Introduction to VLSI Design</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>21-11-2025</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>HS201</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Happiness &amp; Wellbeing</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>21-11-2025</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>EC161</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Digital Design</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>24-11-2025</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>CS261</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Operating Systems</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>24-11-2025</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>DS456</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Machine Learning</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>24-11-2025</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>CS309</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Statistics for CS</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>24-11-2025</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>CS161</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Problem Solving</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>24-11-2025</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>CS262</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Software Design</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>24-11-2025</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>CS303</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Computer Networks</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>24-11-2025</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>DS302</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Computer Communication</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>24-11-2025</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>HS161</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>English Language</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>25-11-2025</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>CS253</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Introduction to AI</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>25-11-2025</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>DS303</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Algorithms and Data Structures</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>25-11-2025</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>EC304</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Signals &amp; Systems</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>25-11-2025</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>PH151</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Introduction to Physics</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>25-11-2025</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>EC303</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Random Processes</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>25-11-2025</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>EC264</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Semiconductor Devices</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>25-11-2025</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>CS463</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Parallel Computing</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>25-11-2025</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CS151</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Introduction to C Programming</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>26-11-2025</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>EC262</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Analog Electronics</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>26-11-2025</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>CS308</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Compiler Design</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>26-11-2025</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>HS157</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Computational Thinking</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>26-11-2025</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>1.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>CS352</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Cryptography &amp; Security</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>26-11-2025</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>HS156</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>Holistic Personality Development</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>27-11-2025</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>1.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>EC355</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Internet of Things</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>27-11-2025</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>NOT ALLOCATED</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>3.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>CS152</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Data Science with Python</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>27-11-2025</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Afternoon</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>14:00 - 17:00</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>HS101</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Environmental Studies</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>28-11-2025</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Morning</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>09:00 - 12:00</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>C004</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>60 students</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2.0 hours</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Parameter</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Maximum Exams Per Day</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Session Duration (minutes)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Include Weekends</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Department Conflict Strictness</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>moderate</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Preference Weight</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Session Balance</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>strict</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Allowed Departments</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>CSE, DSAI, ECE, Mathematics, Physics, Humanities</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Allowed Exam Types</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Theory, Lab</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Additional Rules</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>gapDays, sessionLimit, preferMorning</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Total Exams Scheduled</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Exam Period</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Morning Sessions</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Afternoon Sessions</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Theory Exams</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Lab Exams</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Departments Involved</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>41</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>20-11-2025 to 28-11-2025</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>22</v>
+      </c>
+      <c r="D2" t="n">
+        <v>19</v>
+      </c>
+      <c r="E2" t="n">
+        <v>37</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4</v>
+      </c>
+      <c r="G2" t="n">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Department</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Number of Exams</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Total Duration (min)</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Semesters Involved</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Total Duration (hours)</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>CSE</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>26</v>
+      </c>
+      <c r="C2" t="n">
+        <v>3720</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>DSAI</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ECE</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>1260</v>
+      </c>
+      <c r="D4" t="n">
+        <v>3</v>
+      </c>
+      <c r="E4" t="n">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enhanced classroom allocation logic, adherence of courses to LTPSC structure, configurable exam duration
</commit_message>
<xml_diff>
--- a/backend/output_timetables/exam_schedule_20-11-2025_to_30-11-2025.xlsx
+++ b/backend/output_timetables/exam_schedule_20-11-2025_to_30-11-2025.xlsx
@@ -532,7 +532,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E2" t="n">
@@ -563,7 +563,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -605,11 +605,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -636,7 +636,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -678,7 +678,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E4" t="n">
@@ -709,7 +709,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -751,11 +751,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -782,7 +782,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -824,11 +824,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -855,7 +855,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -897,11 +897,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -970,7 +970,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E8" t="n">
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1043,11 +1043,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1116,7 +1116,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E10" t="n">
@@ -1147,7 +1147,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E11" t="n">
@@ -1220,7 +1220,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1262,11 +1262,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1335,11 +1335,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1408,7 +1408,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E14" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E15" t="n">
@@ -1512,7 +1512,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1554,11 +1554,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1627,11 +1627,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1700,7 +1700,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E18" t="n">
@@ -1731,7 +1731,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1773,11 +1773,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1846,11 +1846,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1919,11 +1919,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1992,11 +1992,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2065,11 +2065,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2211,11 +2211,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2357,7 +2357,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E27" t="n">
@@ -2388,7 +2388,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2430,11 +2430,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2503,11 +2503,11 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -2534,7 +2534,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2576,7 +2576,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E30" t="n">
@@ -2607,7 +2607,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2649,7 +2649,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E31" t="n">
@@ -2680,7 +2680,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2722,7 +2722,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E32" t="n">
@@ -2753,7 +2753,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2795,11 +2795,11 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2868,7 +2868,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E34" t="n">
@@ -2899,7 +2899,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2941,7 +2941,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E35" t="n">
@@ -2972,7 +2972,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3014,11 +3014,11 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3087,11 +3087,11 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>1.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -3118,7 +3118,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3160,11 +3160,11 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -3191,7 +3191,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3233,11 +3233,11 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>1.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>60</v>
+        <v>120</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3306,11 +3306,11 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3379,7 +3379,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E41" t="n">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3452,7 +3452,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E42" t="n">
@@ -3483,7 +3483,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3596,7 +3596,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -3616,7 +3616,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -3757,7 +3757,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -3804,7 +3804,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -3851,7 +3851,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3972,7 +3972,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -3992,7 +3992,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -4086,7 +4086,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -4133,7 +4133,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -4180,7 +4180,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -4227,7 +4227,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4254,7 +4254,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -4274,7 +4274,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4348,7 +4348,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4395,7 +4395,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -4415,7 +4415,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -4462,7 +4462,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -4509,7 +4509,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4583,7 +4583,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -4603,7 +4603,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -4744,7 +4744,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -4791,7 +4791,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4912,7 +4912,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -4932,7 +4932,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -4979,7 +4979,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5006,7 +5006,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -5026,7 +5026,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5053,7 +5053,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -5073,7 +5073,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5100,7 +5100,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -5120,7 +5120,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5194,7 +5194,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -5214,7 +5214,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>1.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -5308,7 +5308,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -5355,7 +5355,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>1.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5382,7 +5382,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -5402,7 +5402,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>3.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5429,7 +5429,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5449,7 +5449,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5496,7 +5496,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2.0 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5548,7 +5548,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
@@ -5772,13 +5772,13 @@
         <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>3720</v>
+        <v>3120</v>
       </c>
       <c r="D2" t="n">
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
@@ -5791,13 +5791,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>1200</v>
+        <v>840</v>
       </c>
       <c r="D3" t="n">
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -5810,13 +5810,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>1260</v>
+        <v>960</v>
       </c>
       <c r="D4" t="n">
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
enhanced course legend with ltpsc structure
</commit_message>
<xml_diff>
--- a/backend/output_timetables/exam_schedule_20-11-2025_to_30-11-2025.xlsx
+++ b/backend/output_timetables/exam_schedule_20-11-2025_to_30-11-2025.xlsx
@@ -532,11 +532,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -563,7 +563,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -605,11 +605,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -636,7 +636,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -678,11 +678,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -709,7 +709,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -751,11 +751,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -782,7 +782,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -824,11 +824,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -855,7 +855,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -897,11 +897,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -970,11 +970,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1043,11 +1043,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1116,11 +1116,11 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1189,11 +1189,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1262,11 +1262,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1335,11 +1335,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1408,11 +1408,11 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1481,11 +1481,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1554,11 +1554,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1627,11 +1627,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1700,11 +1700,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1773,11 +1773,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1846,11 +1846,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1919,11 +1919,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1992,11 +1992,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2065,11 +2065,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2211,11 +2211,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2357,11 +2357,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2430,11 +2430,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2503,11 +2503,11 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -2534,7 +2534,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2576,11 +2576,11 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2649,11 +2649,11 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2722,11 +2722,11 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2795,11 +2795,11 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2868,11 +2868,11 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2941,11 +2941,11 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -2972,7 +2972,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3014,11 +3014,11 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3087,11 +3087,11 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -3118,7 +3118,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3160,11 +3160,11 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -3191,7 +3191,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3233,11 +3233,11 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3306,11 +3306,11 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3379,11 +3379,11 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3452,11 +3452,11 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3596,7 +3596,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -3616,7 +3616,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -3757,7 +3757,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -3804,7 +3804,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -3851,7 +3851,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -3972,7 +3972,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -3992,7 +3992,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -4086,7 +4086,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -4133,7 +4133,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -4180,7 +4180,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -4227,7 +4227,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4254,7 +4254,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -4274,7 +4274,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4348,7 +4348,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4395,7 +4395,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -4415,7 +4415,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -4462,7 +4462,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -4509,7 +4509,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4583,7 +4583,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -4603,7 +4603,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -4744,7 +4744,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -4791,7 +4791,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4912,7 +4912,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -4932,7 +4932,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -4979,7 +4979,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5006,7 +5006,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -5026,7 +5026,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5053,7 +5053,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -5073,7 +5073,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5100,7 +5100,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -5120,7 +5120,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5194,7 +5194,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -5214,7 +5214,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -5308,7 +5308,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -5355,7 +5355,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5382,7 +5382,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -5402,7 +5402,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5429,7 +5429,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>14:00 - 17:00</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5449,7 +5449,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>09:00 - 12:00</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5496,7 +5496,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>2 hours</t>
+          <t>3 hours</t>
         </is>
       </c>
     </row>
@@ -5548,7 +5548,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>120</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4">
@@ -5772,13 +5772,13 @@
         <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>3120</v>
+        <v>4680</v>
       </c>
       <c r="D2" t="n">
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>52</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
@@ -5791,13 +5791,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>840</v>
+        <v>1260</v>
       </c>
       <c r="D3" t="n">
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4">
@@ -5810,13 +5810,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>960</v>
+        <v>1440</v>
       </c>
       <c r="D4" t="n">
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added elective basket B4 for semester 5
</commit_message>
<xml_diff>
--- a/backend/output_timetables/exam_schedule_20-11-2025_to_30-11-2025.xlsx
+++ b/backend/output_timetables/exam_schedule_20-11-2025_to_30-11-2025.xlsx
@@ -532,11 +532,11 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E2" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F2" t="inlineStr">
         <is>
@@ -563,7 +563,7 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
@@ -605,11 +605,11 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E3" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F3" t="inlineStr">
         <is>
@@ -636,7 +636,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -678,11 +678,11 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E4" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F4" t="inlineStr">
         <is>
@@ -709,7 +709,7 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
@@ -751,11 +751,11 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E5" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F5" t="inlineStr">
         <is>
@@ -782,7 +782,7 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
@@ -824,11 +824,11 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E6" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F6" t="inlineStr">
         <is>
@@ -855,7 +855,7 @@
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
@@ -897,11 +897,11 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E7" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F7" t="inlineStr">
         <is>
@@ -928,7 +928,7 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
@@ -970,11 +970,11 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E8" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F8" t="inlineStr">
         <is>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
@@ -1043,11 +1043,11 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E9" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F9" t="inlineStr">
         <is>
@@ -1074,7 +1074,7 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
@@ -1116,11 +1116,11 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E10" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F10" t="inlineStr">
         <is>
@@ -1147,7 +1147,7 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
@@ -1189,11 +1189,11 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E11" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F11" t="inlineStr">
         <is>
@@ -1220,7 +1220,7 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
@@ -1262,11 +1262,11 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E12" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F12" t="inlineStr">
         <is>
@@ -1293,7 +1293,7 @@
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
@@ -1335,11 +1335,11 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E13" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F13" t="inlineStr">
         <is>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
@@ -1408,11 +1408,11 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E14" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F14" t="inlineStr">
         <is>
@@ -1439,7 +1439,7 @@
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
@@ -1481,11 +1481,11 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E15" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F15" t="inlineStr">
         <is>
@@ -1512,7 +1512,7 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
@@ -1554,11 +1554,11 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E16" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F16" t="inlineStr">
         <is>
@@ -1585,7 +1585,7 @@
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
@@ -1627,11 +1627,11 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E17" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F17" t="inlineStr">
         <is>
@@ -1658,7 +1658,7 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
@@ -1700,11 +1700,11 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E18" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F18" t="inlineStr">
         <is>
@@ -1731,7 +1731,7 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
@@ -1773,11 +1773,11 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E19" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F19" t="inlineStr">
         <is>
@@ -1804,7 +1804,7 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
@@ -1846,11 +1846,11 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E20" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F20" t="inlineStr">
         <is>
@@ -1877,7 +1877,7 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
@@ -1919,11 +1919,11 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E21" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F21" t="inlineStr">
         <is>
@@ -1950,7 +1950,7 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
@@ -1992,11 +1992,11 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E22" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F22" t="inlineStr">
         <is>
@@ -2023,7 +2023,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -2065,11 +2065,11 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E23" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F23" t="inlineStr">
         <is>
@@ -2096,7 +2096,7 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
@@ -2138,11 +2138,11 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E24" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F24" t="inlineStr">
         <is>
@@ -2169,7 +2169,7 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
@@ -2211,11 +2211,11 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E25" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F25" t="inlineStr">
         <is>
@@ -2242,7 +2242,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2284,11 +2284,11 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E26" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F26" t="inlineStr">
         <is>
@@ -2315,7 +2315,7 @@
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
@@ -2357,11 +2357,11 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E27" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F27" t="inlineStr">
         <is>
@@ -2388,7 +2388,7 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
@@ -2430,11 +2430,11 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E28" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F28" t="inlineStr">
         <is>
@@ -2461,7 +2461,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2503,11 +2503,11 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E29" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F29" t="inlineStr">
         <is>
@@ -2534,7 +2534,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2576,11 +2576,11 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E30" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F30" t="inlineStr">
         <is>
@@ -2607,7 +2607,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2649,11 +2649,11 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E31" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F31" t="inlineStr">
         <is>
@@ -2680,7 +2680,7 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
@@ -2722,11 +2722,11 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E32" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F32" t="inlineStr">
         <is>
@@ -2753,7 +2753,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2795,11 +2795,11 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E33" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F33" t="inlineStr">
         <is>
@@ -2826,7 +2826,7 @@
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
@@ -2868,11 +2868,11 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E34" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F34" t="inlineStr">
         <is>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
@@ -2941,11 +2941,11 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E35" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F35" t="inlineStr">
         <is>
@@ -2972,7 +2972,7 @@
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
@@ -3014,11 +3014,11 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E36" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F36" t="inlineStr">
         <is>
@@ -3045,7 +3045,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -3087,11 +3087,11 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E37" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F37" t="inlineStr">
         <is>
@@ -3118,7 +3118,7 @@
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
@@ -3160,11 +3160,11 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E38" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F38" t="inlineStr">
         <is>
@@ -3191,7 +3191,7 @@
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
@@ -3233,11 +3233,11 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E39" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F39" t="inlineStr">
         <is>
@@ -3264,7 +3264,7 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
@@ -3306,11 +3306,11 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E40" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F40" t="inlineStr">
         <is>
@@ -3337,7 +3337,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3379,11 +3379,11 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E41" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F41" t="inlineStr">
         <is>
@@ -3410,7 +3410,7 @@
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
@@ -3452,11 +3452,11 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
       <c r="E42" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
       <c r="F42" t="inlineStr">
         <is>
@@ -3483,7 +3483,7 @@
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
@@ -3596,7 +3596,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -3616,7 +3616,7 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3643,7 +3643,7 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
@@ -3663,7 +3663,7 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3690,7 +3690,7 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -3710,7 +3710,7 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3737,7 +3737,7 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -3757,7 +3757,7 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3784,7 +3784,7 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -3804,7 +3804,7 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3831,7 +3831,7 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
@@ -3851,7 +3851,7 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3878,7 +3878,7 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
@@ -3898,7 +3898,7 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3925,7 +3925,7 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -3945,7 +3945,7 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -3972,7 +3972,7 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
@@ -3992,7 +3992,7 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4019,7 +4019,7 @@
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
@@ -4039,7 +4039,7 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4066,7 +4066,7 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -4086,7 +4086,7 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4113,7 +4113,7 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -4133,7 +4133,7 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4160,7 +4160,7 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -4180,7 +4180,7 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4207,7 +4207,7 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -4227,7 +4227,7 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4254,7 +4254,7 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -4274,7 +4274,7 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4301,7 +4301,7 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
@@ -4321,7 +4321,7 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4348,7 +4348,7 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
@@ -4368,7 +4368,7 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4395,7 +4395,7 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -4415,7 +4415,7 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4442,7 +4442,7 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
@@ -4462,7 +4462,7 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4489,7 +4489,7 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
@@ -4509,7 +4509,7 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4536,7 +4536,7 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -4556,7 +4556,7 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4583,7 +4583,7 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
@@ -4603,7 +4603,7 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4630,7 +4630,7 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
@@ -4650,7 +4650,7 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4677,7 +4677,7 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
@@ -4697,7 +4697,7 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4724,7 +4724,7 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
@@ -4744,7 +4744,7 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4771,7 +4771,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -4791,7 +4791,7 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4818,7 +4818,7 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
@@ -4838,7 +4838,7 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4865,7 +4865,7 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
@@ -4885,7 +4885,7 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4912,7 +4912,7 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
@@ -4932,7 +4932,7 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -4959,7 +4959,7 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
@@ -4979,7 +4979,7 @@
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5006,7 +5006,7 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
@@ -5026,7 +5026,7 @@
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5053,7 +5053,7 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -5073,7 +5073,7 @@
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5100,7 +5100,7 @@
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
@@ -5120,7 +5120,7 @@
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5147,7 +5147,7 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
@@ -5167,7 +5167,7 @@
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5194,7 +5194,7 @@
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -5214,7 +5214,7 @@
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5241,7 +5241,7 @@
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
@@ -5261,7 +5261,7 @@
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5288,7 +5288,7 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -5308,7 +5308,7 @@
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
@@ -5355,7 +5355,7 @@
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5382,7 +5382,7 @@
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
@@ -5402,7 +5402,7 @@
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5429,7 +5429,7 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>14:00 - 17:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
@@ -5449,7 +5449,7 @@
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5476,7 +5476,7 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>09:00 - 12:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
@@ -5496,7 +5496,7 @@
       </c>
       <c r="I42" t="inlineStr">
         <is>
-          <t>3 hours</t>
+          <t>2 hours</t>
         </is>
       </c>
     </row>
@@ -5548,7 +5548,7 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>180</v>
+        <v>120</v>
       </c>
     </row>
     <row r="4">
@@ -5772,13 +5772,13 @@
         <v>26</v>
       </c>
       <c r="C2" t="n">
-        <v>4680</v>
+        <v>3120</v>
       </c>
       <c r="D2" t="n">
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>78</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3">
@@ -5791,13 +5791,13 @@
         <v>7</v>
       </c>
       <c r="C3" t="n">
-        <v>1260</v>
+        <v>840</v>
       </c>
       <c r="D3" t="n">
         <v>2</v>
       </c>
       <c r="E3" t="n">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4">
@@ -5810,13 +5810,13 @@
         <v>8</v>
       </c>
       <c r="C4" t="n">
-        <v>1440</v>
+        <v>960</v>
       </c>
       <c r="D4" t="n">
         <v>3</v>
       </c>
       <c r="E4" t="n">
-        <v>24</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added list view for exam schedule preview
</commit_message>
<xml_diff>
--- a/backend/output_timetables/exam_schedule_20-11-2025_to_30-11-2025.xlsx
+++ b/backend/output_timetables/exam_schedule_20-11-2025_to_30-11-2025.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O42"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -736,12 +736,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CS304</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Artificial Intelligence</t>
+          <t>Electronics Theory</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -759,11 +759,11 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>DSAI</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="G5" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -777,17 +777,17 @@
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>23-04-2025</t>
+          <t>16-12-2024</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -797,7 +797,7 @@
       </c>
       <c r="N5" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="O5" t="inlineStr">
@@ -809,12 +809,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>CS263</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Electronics Theory</t>
+          <t>Data Structures</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -832,11 +832,11 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="G6" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -860,7 +860,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>16-12-2024</t>
+          <t>17-12-2024</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -870,7 +870,7 @@
       </c>
       <c r="N6" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="O6" t="inlineStr">
@@ -882,12 +882,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CS263</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Data Structures</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -909,7 +909,7 @@
         </is>
       </c>
       <c r="G7" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -933,7 +933,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>17-12-2024</t>
+          <t>18-12-2024</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -955,12 +955,12 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>DS161</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Statistics</t>
+          <t>Introduction to Programming</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -986,27 +986,27 @@
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>18-12-2024</t>
+          <t>19-12-2024</t>
         </is>
       </c>
       <c r="M8" t="inlineStr">
@@ -1016,7 +1016,7 @@
       </c>
       <c r="N8" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="O8" t="inlineStr">
@@ -1028,12 +1028,12 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DA262</t>
+          <t>MA261</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Data Handling</t>
+          <t>Differential Equations</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -1051,7 +1051,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>DSAI</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="G9" t="n">
@@ -1059,27 +1059,27 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>22-04-2025</t>
+          <t>15-04-2025</t>
         </is>
       </c>
       <c r="M9" t="inlineStr">
@@ -1101,12 +1101,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>DA262</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Introduction to Programming</t>
+          <t>Data Handling</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -1124,11 +1124,11 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>DSAI</t>
         </is>
       </c>
       <c r="G10" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -1152,7 +1152,7 @@
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>19-12-2024</t>
+          <t>22-04-2025</t>
         </is>
       </c>
       <c r="M10" t="inlineStr">
@@ -1162,7 +1162,7 @@
       </c>
       <c r="N10" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="O10" t="inlineStr">
@@ -1174,12 +1174,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MA261</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Differential Equations</t>
+          <t>Probability</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1201,7 +1201,7 @@
         </is>
       </c>
       <c r="G11" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1215,17 +1215,17 @@
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>15-04-2025</t>
+          <t>20-12-2024</t>
         </is>
       </c>
       <c r="M11" t="inlineStr">
@@ -1235,7 +1235,7 @@
       </c>
       <c r="N11" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="O11" t="inlineStr">
@@ -1247,12 +1247,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CS307</t>
+          <t>MA262</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Machine Learning</t>
+          <t>Multivariable Calculus</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1270,7 +1270,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>DSAI</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="G12" t="n">
@@ -1288,17 +1288,17 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>24-04-2025</t>
+          <t>16-04-2025</t>
         </is>
       </c>
       <c r="M12" t="inlineStr">
@@ -1320,12 +1320,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EC301</t>
+          <t>CS304</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Digital Signal Processing</t>
+          <t>Artificial Intelligence</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1343,7 +1343,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>DSAI</t>
         </is>
       </c>
       <c r="G13" t="n">
@@ -1361,17 +1361,17 @@
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>25-04-2025</t>
+          <t>23-04-2025</t>
         </is>
       </c>
       <c r="M13" t="inlineStr">
@@ -1393,12 +1393,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>Digital Design</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1424,27 +1424,27 @@
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>20-12-2024</t>
+          <t>21-12-2024</t>
         </is>
       </c>
       <c r="M14" t="inlineStr">
@@ -1466,12 +1466,12 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MA262</t>
+          <t>CS261</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Multivariable Calculus</t>
+          <t>Operating Systems</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1497,27 +1497,27 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>16-04-2025</t>
+          <t>17-04-2025</t>
         </is>
       </c>
       <c r="M15" t="inlineStr">
@@ -1539,12 +1539,12 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>EC302</t>
+          <t>CS307</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Introduction to VLSI Design</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1562,7 +1562,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>DSAI</t>
         </is>
       </c>
       <c r="G16" t="n">
@@ -1570,27 +1570,27 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>26-04-2025</t>
+          <t>24-04-2025</t>
         </is>
       </c>
       <c r="M16" t="inlineStr">
@@ -1612,12 +1612,12 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HS201</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Happiness &amp; Wellbeing</t>
+          <t>Problem Solving</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1635,20 +1635,20 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Monday</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1663,7 +1663,7 @@
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>28-04-2025</t>
+          <t>22-12-2024</t>
         </is>
       </c>
       <c r="M17" t="inlineStr">
@@ -1673,7 +1673,7 @@
       </c>
       <c r="N17" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="O17" t="inlineStr">
@@ -1685,12 +1685,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>CS262</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Digital Design</t>
+          <t>Software Design</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1712,7 +1712,7 @@
         </is>
       </c>
       <c r="G18" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1726,17 +1726,17 @@
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>21-12-2024</t>
+          <t>18-04-2025</t>
         </is>
       </c>
       <c r="M18" t="inlineStr">
@@ -1746,7 +1746,7 @@
       </c>
       <c r="N18" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="O18" t="inlineStr">
@@ -1758,12 +1758,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CS261</t>
+          <t>EC301</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Operating Systems</t>
+          <t>Digital Signal Processing</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1781,7 +1781,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="G19" t="n">
@@ -1799,17 +1799,17 @@
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>17-04-2025</t>
+          <t>25-04-2025</t>
         </is>
       </c>
       <c r="M19" t="inlineStr">
@@ -1831,12 +1831,12 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DS456</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Machine Learning</t>
+          <t>English Language</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1854,20 +1854,20 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>DSAI</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>16-05-2025</t>
+          <t>23-12-2024</t>
         </is>
       </c>
       <c r="M20" t="inlineStr">
@@ -1892,7 +1892,7 @@
       </c>
       <c r="N20" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="O20" t="inlineStr">
@@ -1904,12 +1904,12 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CS309</t>
+          <t>EC302</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Statistics for CS</t>
+          <t>Introduction to VLSI Design</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1927,20 +1927,20 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1955,7 +1955,7 @@
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>17-05-2025</t>
+          <t>26-04-2025</t>
         </is>
       </c>
       <c r="M21" t="inlineStr">
@@ -1977,12 +1977,12 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>HS201</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Problem Solving</t>
+          <t>Happiness &amp; Wellbeing</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -2000,35 +2000,35 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>22-12-2024</t>
+          <t>28-04-2025</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
@@ -2038,7 +2038,7 @@
       </c>
       <c r="N22" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="O22" t="inlineStr">
@@ -2050,12 +2050,12 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CS262</t>
+          <t>PH151</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Software Design</t>
+          <t>Introduction to Physics</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -2077,16 +2077,16 @@
         </is>
       </c>
       <c r="G23" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -2101,7 +2101,7 @@
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>18-04-2025</t>
+          <t>24-12-2024</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
@@ -2111,7 +2111,7 @@
       </c>
       <c r="N23" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="O23" t="inlineStr">
@@ -2123,12 +2123,12 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CS303</t>
+          <t>CS253</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Computer Networks</t>
+          <t>Introduction to AI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -2150,16 +2150,16 @@
         </is>
       </c>
       <c r="G24" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2174,7 +2174,7 @@
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>18-05-2025</t>
+          <t>29-04-2025</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
@@ -2196,12 +2196,12 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DS302</t>
+          <t>DS456</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Computer Communication</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -2227,12 +2227,12 @@
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>Monday</t>
+          <t>Tuesday</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2247,7 +2247,7 @@
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>21-05-2025</t>
+          <t>16-05-2025</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
@@ -2269,17 +2269,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>CS151</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>English Language</t>
+          <t>Introduction to C Programming</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Theory</t>
+          <t>Lab</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -2300,12 +2300,12 @@
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2320,7 +2320,7 @@
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>23-12-2024</t>
+          <t>25-12-2024</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
@@ -2342,12 +2342,12 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CS253</t>
+          <t>CS309</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Introduction to AI</t>
+          <t>Statistics for CS</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -2369,16 +2369,16 @@
         </is>
       </c>
       <c r="G27" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2393,7 +2393,7 @@
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>29-04-2025</t>
+          <t>17-05-2025</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
@@ -2415,12 +2415,12 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DS303</t>
+          <t>DS302</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Algorithms and Data Structures</t>
+          <t>Computer Communication</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -2446,12 +2446,12 @@
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2466,7 +2466,7 @@
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>22-05-2025</t>
+          <t>21-05-2025</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
@@ -2488,12 +2488,12 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>EC304</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Signals &amp; Systems</t>
+          <t>Computational Thinking</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -2511,35 +2511,35 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>25-05-2025</t>
+          <t>26-12-2024</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
@@ -2549,7 +2549,7 @@
       </c>
       <c r="N29" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="O29" t="inlineStr">
@@ -2561,12 +2561,12 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>CS303</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Introduction to Physics</t>
+          <t>Computer Networks</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2588,16 +2588,16 @@
         </is>
       </c>
       <c r="G30" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2612,7 +2612,7 @@
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>24-12-2024</t>
+          <t>18-05-2025</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
@@ -2622,7 +2622,7 @@
       </c>
       <c r="N30" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="O30" t="inlineStr">
@@ -2634,12 +2634,12 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>EC303</t>
+          <t>DS303</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Random Processes</t>
+          <t>Algorithms and Data Structures</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2657,7 +2657,7 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>DSAI</t>
         </is>
       </c>
       <c r="G31" t="n">
@@ -2665,12 +2665,12 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Wednesday</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2685,7 +2685,7 @@
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>24-05-2025</t>
+          <t>22-05-2025</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
@@ -2707,12 +2707,12 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>EC264</t>
+          <t>HS156</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Semiconductor Devices</t>
+          <t>Holistic Personality Development</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2730,35 +2730,35 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>26-05-2025</t>
+          <t>27-12-2024</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
@@ -2768,7 +2768,7 @@
       </c>
       <c r="N32" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="O32" t="inlineStr">
@@ -2780,12 +2780,12 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CS463</t>
+          <t>EC303</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Parallel Computing</t>
+          <t>Random Processes</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
@@ -2803,7 +2803,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="G33" t="n">
@@ -2811,27 +2811,27 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
         <is>
-          <t>Tuesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>29-05-2025</t>
+          <t>24-05-2025</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
@@ -2853,17 +2853,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>EC264</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Introduction to C Programming</t>
+          <t>Semiconductor Devices</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Lab</t>
+          <t>Theory</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -2876,20 +2876,20 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2904,7 +2904,7 @@
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>25-12-2024</t>
+          <t>26-05-2025</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="N34" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="O34" t="inlineStr">
@@ -2926,17 +2926,17 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>EC262</t>
+          <t>CS152</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Analog Electronics</t>
+          <t>Data Science with Python</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Theory</t>
+          <t>Lab</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -2949,35 +2949,35 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>27-05-2025</t>
+          <t>30-04-2025</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
@@ -2987,7 +2987,7 @@
       </c>
       <c r="N35" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="O35" t="inlineStr">
@@ -2999,12 +2999,12 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CS308</t>
+          <t>EC304</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Compiler Design</t>
+          <t>Signals &amp; Systems</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -3022,7 +3022,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="G36" t="n">
@@ -3030,27 +3030,27 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>30-05-2025</t>
+          <t>25-05-2025</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
@@ -3072,12 +3072,12 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>EC262</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Computational Thinking</t>
+          <t>Analog Electronics</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
@@ -3095,20 +3095,20 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -3123,7 +3123,7 @@
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>26-12-2024</t>
+          <t>27-05-2025</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
@@ -3133,7 +3133,7 @@
       </c>
       <c r="N37" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="O37" t="inlineStr">
@@ -3145,12 +3145,12 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CS352</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Cryptography &amp; Security</t>
+          <t>Environmental Studies</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
@@ -3176,27 +3176,27 @@
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="I38" t="inlineStr">
         <is>
-          <t>Wednesday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>31-05-2025</t>
+          <t>20-05-2025</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
@@ -3206,7 +3206,7 @@
       </c>
       <c r="N38" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="O38" t="inlineStr">
@@ -3218,12 +3218,12 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>CS463</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Holistic Personality Development</t>
+          <t>Parallel Computing</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -3245,16 +3245,16 @@
         </is>
       </c>
       <c r="G39" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="I39" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
@@ -3269,7 +3269,7 @@
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>27-12-2024</t>
+          <t>29-05-2025</t>
         </is>
       </c>
       <c r="M39" t="inlineStr">
@@ -3279,7 +3279,7 @@
       </c>
       <c r="N39" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="O39" t="inlineStr">
@@ -3291,12 +3291,12 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>EC355</t>
+          <t>CS352</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Internet of Things</t>
+          <t>Cryptography &amp; Security</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
@@ -3322,12 +3322,12 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>01-06-2025</t>
+          <t>31-05-2025</t>
         </is>
       </c>
       <c r="M40" t="inlineStr">
@@ -3364,17 +3364,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CS152</t>
+          <t>CS308</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Data Science with Python</t>
+          <t>Compiler Design</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Lab</t>
+          <t>Theory</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -3391,16 +3391,16 @@
         </is>
       </c>
       <c r="G41" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="I41" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3415,7 +3415,7 @@
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>30-04-2025</t>
+          <t>30-05-2025</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
@@ -3429,79 +3429,6 @@
         </is>
       </c>
       <c r="O41" t="inlineStr">
-        <is>
-          <t>60 students</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>HS101</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Environmental Studies</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Theory</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>2 hours</t>
-        </is>
-      </c>
-      <c r="E42" t="n">
-        <v>120</v>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>CSE</t>
-        </is>
-      </c>
-      <c r="G42" t="n">
-        <v>5</v>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>28-11-2025</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
-        <is>
-          <t>Friday</t>
-        </is>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="K42" t="inlineStr">
-        <is>
-          <t>09:00 - 11:00</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>20-05-2025</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>Scheduled</t>
-        </is>
-      </c>
-      <c r="N42" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="O42" t="inlineStr">
         <is>
           <t>60 students</t>
         </is>
@@ -3518,7 +3445,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3717,12 +3644,12 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CS304</t>
+          <t>EC101</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Artificial Intelligence</t>
+          <t>Electronics Theory</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -3732,17 +3659,17 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -3752,7 +3679,7 @@
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>DSAI</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -3764,12 +3691,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>EC101</t>
+          <t>CS263</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Electronics Theory</t>
+          <t>Data Structures</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -3789,7 +3716,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -3799,7 +3726,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -3811,12 +3738,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CS263</t>
+          <t>MA161</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Data Structures</t>
+          <t>Statistics</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -3858,32 +3785,32 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MA161</t>
+          <t>DS161</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Statistics</t>
+          <t>Introduction to Programming</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -3905,27 +3832,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DA262</t>
+          <t>MA261</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Data Handling</t>
+          <t>Differential Equations</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>20-11-2025</t>
+          <t>21-11-2025</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -3940,7 +3867,7 @@
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>DSAI</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -3952,12 +3879,12 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>DS161</t>
+          <t>DA262</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Introduction to Programming</t>
+          <t>Data Handling</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -3977,7 +3904,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -3987,7 +3914,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>DSAI</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -3999,12 +3926,12 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>MA261</t>
+          <t>MA162</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Differential Equations</t>
+          <t>Probability</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -4014,17 +3941,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -4046,12 +3973,12 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CS307</t>
+          <t>MA262</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Machine Learning</t>
+          <t>Multivariable Calculus</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -4061,12 +3988,12 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
@@ -4081,7 +4008,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>DSAI</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -4093,12 +4020,12 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>EC301</t>
+          <t>CS304</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Digital Signal Processing</t>
+          <t>Artificial Intelligence</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -4108,12 +4035,12 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
@@ -4128,7 +4055,7 @@
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>DSAI</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -4140,27 +4067,27 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>MA162</t>
+          <t>EC161</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Probability</t>
+          <t>Digital Design</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
@@ -4187,27 +4114,27 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>MA262</t>
+          <t>CS261</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Multivariable Calculus</t>
+          <t>Operating Systems</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -4234,27 +4161,27 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>EC302</t>
+          <t>CS307</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Introduction to VLSI Design</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
@@ -4269,7 +4196,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>DSAI</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -4281,17 +4208,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>HS201</t>
+          <t>CS161</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Happiness &amp; Wellbeing</t>
+          <t>Problem Solving</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>21-11-2025</t>
+          <t>24-11-2025</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -4306,7 +4233,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -4316,7 +4243,7 @@
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -4328,12 +4255,12 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>EC161</t>
+          <t>CS262</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Digital Design</t>
+          <t>Software Design</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -4343,17 +4270,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -4375,12 +4302,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CS261</t>
+          <t>EC301</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Operating Systems</t>
+          <t>Digital Signal Processing</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -4390,12 +4317,12 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
@@ -4410,7 +4337,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -4422,17 +4349,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>DS456</t>
+          <t>HS161</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Machine Learning</t>
+          <t>English Language</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -4447,7 +4374,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -4457,7 +4384,7 @@
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>DSAI</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -4469,17 +4396,17 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CS309</t>
+          <t>EC302</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Statistics for CS</t>
+          <t>Introduction to VLSI Design</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -4504,7 +4431,7 @@
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -4516,32 +4443,32 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CS161</t>
+          <t>HS201</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Problem Solving</t>
+          <t>Happiness &amp; Wellbeing</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -4551,7 +4478,7 @@
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -4563,17 +4490,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CS262</t>
+          <t>PH151</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Software Design</t>
+          <t>Introduction to Physics</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -4588,7 +4515,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -4610,17 +4537,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CS303</t>
+          <t>CS253</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Computer Networks</t>
+          <t>Introduction to AI</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -4657,17 +4584,17 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>DS302</t>
+          <t>DS456</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Computer Communication</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>24-11-2025</t>
+          <t>25-11-2025</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
@@ -4704,17 +4631,17 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>HS161</t>
+          <t>CS151</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>English Language</t>
+          <t>Introduction to C Programming</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -4751,17 +4678,17 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CS253</t>
+          <t>CS309</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Introduction to AI</t>
+          <t>Statistics for CS</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -4798,17 +4725,17 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>DS303</t>
+          <t>DS302</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Algorithms and Data Structures</t>
+          <t>Computer Communication</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
@@ -4845,32 +4772,32 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>EC304</t>
+          <t>HS157</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Signals &amp; Systems</t>
+          <t>Computational Thinking</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -4880,7 +4807,7 @@
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -4892,17 +4819,17 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>PH151</t>
+          <t>CS303</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Introduction to Physics</t>
+          <t>Computer Networks</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -4917,7 +4844,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -4939,17 +4866,17 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>EC303</t>
+          <t>DS303</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Random Processes</t>
+          <t>Algorithms and Data Structures</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>26-11-2025</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -4974,7 +4901,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>DSAI</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -4986,32 +4913,32 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>EC264</t>
+          <t>HS156</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Semiconductor Devices</t>
+          <t>Holistic Personality Development</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -5021,7 +4948,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -5033,27 +4960,27 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CS463</t>
+          <t>EC303</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Parallel Computing</t>
+          <t>Random Processes</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>25-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
@@ -5068,7 +4995,7 @@
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="I33" t="inlineStr">
@@ -5080,17 +5007,17 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CS151</t>
+          <t>EC264</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Introduction to C Programming</t>
+          <t>Semiconductor Devices</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -5105,7 +5032,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -5115,7 +5042,7 @@
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="I34" t="inlineStr">
@@ -5127,32 +5054,32 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>EC262</t>
+          <t>CS152</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Analog Electronics</t>
+          <t>Data Science with Python</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -5162,7 +5089,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>ECE</t>
+          <t>CSE</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -5174,27 +5101,27 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CS308</t>
+          <t>EC304</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Compiler Design</t>
+          <t>Signals &amp; Systems</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Morning</t>
+          <t>Afternoon</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>09:00 - 11:00</t>
+          <t>14:00 - 16:00</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
@@ -5209,7 +5136,7 @@
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="I36" t="inlineStr">
@@ -5221,17 +5148,17 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>HS157</t>
+          <t>EC262</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Computational Thinking</t>
+          <t>Analog Electronics</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>27-11-2025</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -5246,7 +5173,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -5256,7 +5183,7 @@
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>CSE</t>
+          <t>ECE</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -5268,32 +5195,32 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CS352</t>
+          <t>HS101</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Cryptography &amp; Security</t>
+          <t>Environmental Studies</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>26-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Afternoon</t>
+          <t>Morning</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>14:00 - 16:00</t>
+          <t>09:00 - 11:00</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>NOT ALLOCATED</t>
+          <t>C004</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -5315,17 +5242,17 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>HS156</t>
+          <t>CS463</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Holistic Personality Development</t>
+          <t>Parallel Computing</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -5340,7 +5267,7 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>C004</t>
+          <t>NOT ALLOCATED</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -5362,17 +5289,17 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>EC355</t>
+          <t>CS352</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Internet of Things</t>
+          <t>Cryptography &amp; Security</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -5409,17 +5336,17 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CS152</t>
+          <t>CS308</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Data Science with Python</t>
+          <t>Compiler Design</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>27-11-2025</t>
+          <t>28-11-2025</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -5448,53 +5375,6 @@
         </is>
       </c>
       <c r="I41" t="inlineStr">
-        <is>
-          <t>2 hours</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>HS101</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Environmental Studies</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>28-11-2025</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Morning</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>09:00 - 11:00</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>C004</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>60 students</t>
-        </is>
-      </c>
-      <c r="H42" t="inlineStr">
-        <is>
-          <t>CSE</t>
-        </is>
-      </c>
-      <c r="I42" t="inlineStr">
         <is>
           <t>2 hours</t>
         </is>
@@ -5538,7 +5418,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3">
@@ -5693,7 +5573,7 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -5701,13 +5581,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" t="n">
         <v>19</v>
       </c>
       <c r="E2" t="n">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" t="n">
         <v>4</v>
@@ -5769,16 +5649,16 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C2" t="n">
-        <v>3120</v>
+        <v>3000</v>
       </c>
       <c r="D2" t="n">
         <v>3</v>
       </c>
       <c r="E2" t="n">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3">

</xml_diff>